<commit_message>
change and upadate in add,view,view.py,super user view
</commit_message>
<xml_diff>
--- a/media/reports/Store Item.xlsx
+++ b/media/reports/Store Item.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,22 +451,211 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Store 1</t>
+          <t>store 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>S/MAX 22" GUARD</t>
+          <t>Blade</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>2000</v>
       </c>
       <c r="D2" t="n">
+        <v>1626</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SKICROP TRINITY PVT LTD</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Blade</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" t="n">
+        <v>500</v>
+      </c>
+      <c r="E3" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>store 1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Fitting Screw</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5003</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5003</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SKICROP TRINITY PVT LTD</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Fitting Screw</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>200</v>
+      </c>
+      <c r="D5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>store 1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PVC Socket</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4800</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>store 1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Side Knob (S/Max, Max, Farata)</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>2000</v>
       </c>
-      <c r="E2" t="n">
-        <v>2000</v>
+      <c r="D7" t="n">
+        <v>1700</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SKICROP TRINITY PVT LTD</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PVC Socket</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>200</v>
+      </c>
+      <c r="D8" t="n">
+        <v>200</v>
+      </c>
+      <c r="E8" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SKICROP TRINITY PVT LTD</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Side Knob (S/Max, Max, Farata)</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" t="n">
+        <v>300</v>
+      </c>
+      <c r="E9" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>store 1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Box</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>store 1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Pink Tape 6mm X 55 Mts</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>33</v>
+      </c>
+      <c r="D11" t="n">
+        <v>33</v>
+      </c>
+      <c r="E11" t="n">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>